<commit_message>
captured image upload option added
</commit_message>
<xml_diff>
--- a/commands/adatok.xlsx
+++ b/commands/adatok.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Típus</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Mályva csillámos tüllös body, használtan vásárolt</t>
+  </si>
+  <si>
+    <t>Ágynemű</t>
+  </si>
+  <si>
+    <t>Probakép</t>
+  </si>
+  <si>
+    <t>64-110</t>
+  </si>
+  <si>
+    <t>2023-05-13</t>
   </si>
 </sst>
 </file>
@@ -432,7 +444,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +599,27 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Issue #1 and #2 fixed
</commit_message>
<xml_diff>
--- a/commands/adatok.xlsx
+++ b/commands/adatok.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Típus</t>
   </si>
@@ -95,16 +95,43 @@
     <t>Mályva csillámos tüllös body, használtan vásárolt</t>
   </si>
   <si>
-    <t>Ágynemű</t>
-  </si>
-  <si>
-    <t>Probakép</t>
-  </si>
-  <si>
-    <t>64-110</t>
-  </si>
-  <si>
-    <t>2023-05-13</t>
+    <t>Ruha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kantáros farmer </t>
+  </si>
+  <si>
+    <t>Kantáros farmer ruha csíkos bodyval, új</t>
+  </si>
+  <si>
+    <t>2023-05-15</t>
+  </si>
+  <si>
+    <t>Felső</t>
+  </si>
+  <si>
+    <t>Rózsaszín szett</t>
+  </si>
+  <si>
+    <t>Rózsaszín átlapolt felső nadrággal és sapkával, új</t>
+  </si>
+  <si>
+    <t>Mályva overál</t>
+  </si>
+  <si>
+    <t>Mályva színű,bundás overál</t>
+  </si>
+  <si>
+    <t>Dóri, Krisztián</t>
+  </si>
+  <si>
+    <t>Hálózsák</t>
+  </si>
+  <si>
+    <t>Vonatos hálózsák</t>
+  </si>
+  <si>
+    <t>Vastag, vonat mintás hálózsák</t>
   </si>
 </sst>
 </file>
@@ -444,7 +471,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,17 +633,88 @@
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="D7"/>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
       <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
db connection modification, seperate css files
</commit_message>
<xml_diff>
--- a/commands/adatok.xlsx
+++ b/commands/adatok.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="374">
   <si>
     <t>Típus</t>
   </si>
@@ -116,6 +116,9 @@
     <t>Rózsaszín átlapolt felső nadrággal és sapkával, új</t>
   </si>
   <si>
+    <t>Overál</t>
+  </si>
+  <si>
     <t>Mályva overál</t>
   </si>
   <si>
@@ -963,6 +966,177 @@
   </si>
   <si>
     <t>Többféle vékony anyagú sapka, lsd fénykép</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rózsaszín decathlonos alig használt cipő </t>
+  </si>
+  <si>
+    <t>Márk, Niki</t>
+  </si>
+  <si>
+    <t>2023-06-04</t>
+  </si>
+  <si>
+    <t>Magenta nike</t>
+  </si>
+  <si>
+    <t>Magenta színű bebújos Nike cipő</t>
+  </si>
+  <si>
+    <t>Narancssárga</t>
+  </si>
+  <si>
+    <t>Narancssárga vastag bélelr overál</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rózsaszín pöttyös </t>
+  </si>
+  <si>
+    <t>Sötétkék, rózsaszín pöttyös overál, vékonyabb</t>
+  </si>
+  <si>
+    <t>Pillangós</t>
+  </si>
+  <si>
+    <t>Kék színű pillangó mintás overál, méret nem látszik</t>
+  </si>
+  <si>
+    <t>Babarózsaszín macis</t>
+  </si>
+  <si>
+    <t>80-86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rózsaszín maci mintás vastag overál, méret nem látszik </t>
+  </si>
+  <si>
+    <t>Pink egeres</t>
+  </si>
+  <si>
+    <t>Pink egér mintás overál</t>
+  </si>
+  <si>
+    <t>Rózsaszín pillangós ruha</t>
+  </si>
+  <si>
+    <t>Pöttyös csipkés</t>
+  </si>
+  <si>
+    <t>Rózsaszín felső fekete pöttyökkel, alul fehér tüllös és csipkés</t>
+  </si>
+  <si>
+    <t>Fehér mintás</t>
+  </si>
+  <si>
+    <t>Fehér alapon mintás, állatok és szivárvány, van hozzá nadrág is</t>
+  </si>
+  <si>
+    <t>Smiley</t>
+  </si>
+  <si>
+    <t>Piros színű smiley-s pulcsi</t>
+  </si>
+  <si>
+    <t>Drapp szett</t>
+  </si>
+  <si>
+    <t>Drapp színű pulcsi hozzá tartozó nadrággal</t>
+  </si>
+  <si>
+    <t>Ujjatlan mosómedvés</t>
+  </si>
+  <si>
+    <t>Ujjatlan mosómedvés rugdalózó, zokni nélküli</t>
+  </si>
+  <si>
+    <t>Zöld Piros macis</t>
+  </si>
+  <si>
+    <t>Rövid ujjú body, zöld-piros mintával</t>
+  </si>
+  <si>
+    <t>Denevéres szett</t>
+  </si>
+  <si>
+    <t>Fekete denevéres szett, hozzá tartozó sapival és nadrággal</t>
+  </si>
+  <si>
+    <t>Szürke egeres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szürke vastag kantáros nadrág, méret nem látszik </t>
+  </si>
+  <si>
+    <t>Sárga</t>
+  </si>
+  <si>
+    <t>Sárga vastag átlapolós pulcsi</t>
+  </si>
+  <si>
+    <t>Fehér vékony pulcsi, minta nélküli patentnál kicsi folt</t>
+  </si>
+  <si>
+    <t>Csillagos</t>
+  </si>
+  <si>
+    <t>Fehér alapon csillag mintás vastag rugi</t>
+  </si>
+  <si>
+    <t>Pasztel zöld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasztel zöld minta nélküli nadrág </t>
+  </si>
+  <si>
+    <t>Micimackós</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vékony micimackós rugdalózó </t>
+  </si>
+  <si>
+    <t>Csíkos macis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vastag barna csíkos macis rugdalózó </t>
+  </si>
+  <si>
+    <t>Plüssös átlapolós</t>
+  </si>
+  <si>
+    <t>Fehér minta nélküli plüssös átlapolós</t>
+  </si>
+  <si>
+    <t>Kék százlábús</t>
+  </si>
+  <si>
+    <t>Fehér alapon kék bogaras body, 2 db</t>
+  </si>
+  <si>
+    <t>Kék csillagos</t>
+  </si>
+  <si>
+    <t>Fehér alapon kék csillagos body, méret nem látszik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sárga csíkos rugdalózó micimackós </t>
+  </si>
+  <si>
+    <t>Fehér mosómedvés</t>
+  </si>
+  <si>
+    <t>Ujjatlan fehér vastag mosómedvés rugdalózó</t>
+  </si>
+  <si>
+    <t>Little sweet heart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kék vastag feliratos rugdalózó </t>
+  </si>
+  <si>
+    <t>56-62</t>
+  </si>
+  <si>
+    <t>Fehér rövid ujjú body minta nélküli, mellénél folt</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1476,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G138"/>
+  <dimension ref="A1:G167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1505,22 +1679,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9">
         <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -1528,22 +1702,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
         <v>29</v>
@@ -1551,508 +1725,508 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11">
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18">
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19">
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21">
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
         <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
         <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
         <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
         <v>17</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25">
         <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
         <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
         <v>17</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E29" t="s">
         <v>17</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C30">
         <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C31">
         <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
         <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32">
         <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E32" t="s">
         <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2060,22 +2234,22 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33">
         <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2083,22 +2257,22 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C34">
         <v>56</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2106,22 +2280,22 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35">
         <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
         <v>17</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2129,22 +2303,22 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C36">
         <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E36" t="s">
         <v>17</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2152,22 +2326,22 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C37">
         <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E37" t="s">
         <v>17</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2175,45 +2349,45 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C38">
         <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E38" t="s">
         <v>17</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C39">
         <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
         <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2221,59 +2395,59 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E40" t="s">
         <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
         <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -2282,21 +2456,21 @@
         <v>11</v>
       </c>
       <c r="G42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E43" t="s">
         <v>17</v>
@@ -2305,21 +2479,21 @@
         <v>18</v>
       </c>
       <c r="G43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E44" t="s">
         <v>17</v>
@@ -2328,21 +2502,21 @@
         <v>18</v>
       </c>
       <c r="G44" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -2351,113 +2525,113 @@
         <v>11</v>
       </c>
       <c r="G45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D46" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G46" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" t="s">
+        <v>124</v>
+      </c>
+      <c r="D47" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" t="s">
         <v>121</v>
       </c>
-      <c r="B47" t="s">
-        <v>122</v>
-      </c>
-      <c r="C47" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" t="s">
-        <v>124</v>
-      </c>
-      <c r="E47" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" t="s">
-        <v>120</v>
-      </c>
       <c r="G47" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" t="s">
         <v>121</v>
       </c>
-      <c r="B48" t="s">
-        <v>125</v>
-      </c>
-      <c r="C48" t="s">
-        <v>123</v>
-      </c>
-      <c r="D48" t="s">
-        <v>126</v>
-      </c>
-      <c r="E48" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" t="s">
-        <v>120</v>
-      </c>
       <c r="G48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" t="s">
         <v>121</v>
       </c>
-      <c r="B49" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" t="s">
-        <v>17</v>
-      </c>
-      <c r="F49" t="s">
-        <v>120</v>
-      </c>
       <c r="G49" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -2466,21 +2640,21 @@
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -2489,21 +2663,21 @@
         <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C52">
         <v>68</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -2512,21 +2686,21 @@
         <v>11</v>
       </c>
       <c r="G52" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
@@ -2535,21 +2709,21 @@
         <v>11</v>
       </c>
       <c r="G53" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D54" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
@@ -2558,21 +2732,21 @@
         <v>11</v>
       </c>
       <c r="G54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E55" t="s">
         <v>10</v>
@@ -2581,21 +2755,21 @@
         <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C56">
         <v>56</v>
       </c>
       <c r="D56" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E56" t="s">
         <v>10</v>
@@ -2604,7 +2778,7 @@
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2612,13 +2786,13 @@
         <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C57">
         <v>68</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E57" t="s">
         <v>10</v>
@@ -2627,7 +2801,7 @@
         <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2635,13 +2809,13 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C58">
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E58" t="s">
         <v>10</v>
@@ -2650,7 +2824,7 @@
         <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2658,13 +2832,13 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C59">
         <v>56</v>
       </c>
       <c r="D59" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E59" t="s">
         <v>10</v>
@@ -2673,168 +2847,168 @@
         <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C60">
         <v>62</v>
       </c>
       <c r="D60" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E60" t="s">
         <v>17</v>
       </c>
       <c r="F60" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G60" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E61" t="s">
         <v>17</v>
       </c>
       <c r="F61" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G61" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E62" t="s">
         <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G62" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E63" t="s">
         <v>17</v>
       </c>
       <c r="F63" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G63" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B64" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C64">
         <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E64" t="s">
         <v>17</v>
       </c>
       <c r="F64" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G64" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B65" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C65">
         <v>68</v>
       </c>
       <c r="D65" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E65" t="s">
         <v>17</v>
       </c>
       <c r="F65" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G65" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C66">
         <v>62</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E66" t="s">
         <v>17</v>
       </c>
       <c r="F66" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G66" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2842,45 +3016,45 @@
         <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C67" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D67" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E67" t="s">
         <v>17</v>
       </c>
       <c r="F67" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G67" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B68" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C68" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D68" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E68" t="s">
         <v>17</v>
       </c>
       <c r="F68" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G68" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2888,22 +3062,22 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C69">
         <v>62</v>
       </c>
       <c r="D69" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E69" t="s">
         <v>17</v>
       </c>
       <c r="F69" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G69" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2911,22 +3085,22 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E70" t="s">
         <v>17</v>
       </c>
       <c r="F70" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G70" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2934,45 +3108,45 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D71" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E71" t="s">
         <v>17</v>
       </c>
       <c r="F71" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G71" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B72" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C72" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D72" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E72" t="s">
         <v>17</v>
       </c>
       <c r="F72" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G72" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2980,68 +3154,68 @@
         <v>26</v>
       </c>
       <c r="B73" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C73">
         <v>62</v>
       </c>
       <c r="D73" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E73" t="s">
         <v>17</v>
       </c>
       <c r="F73" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G73" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C74">
         <v>62</v>
       </c>
       <c r="D74" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
         <v>17</v>
       </c>
       <c r="F74" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G74" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B75" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C75" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D75" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E75" t="s">
         <v>17</v>
       </c>
       <c r="F75" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3049,22 +3223,22 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C76">
         <v>62</v>
       </c>
       <c r="D76" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E76" t="s">
         <v>17</v>
       </c>
       <c r="F76" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G76" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3072,22 +3246,22 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C77">
         <v>56</v>
       </c>
       <c r="D77" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E77" t="s">
         <v>17</v>
       </c>
       <c r="F77" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G77" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3095,22 +3269,22 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C78">
         <v>56</v>
       </c>
       <c r="D78" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E78" t="s">
         <v>17</v>
       </c>
       <c r="F78" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G78" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3118,45 +3292,45 @@
         <v>30</v>
       </c>
       <c r="B79" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C79">
         <v>56</v>
       </c>
       <c r="D79" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E79" t="s">
         <v>17</v>
       </c>
       <c r="F79" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G79" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B80" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C80" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D80" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E80" t="s">
         <v>17</v>
       </c>
       <c r="F80" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G80" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3164,22 +3338,22 @@
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C81">
         <v>62</v>
       </c>
       <c r="D81" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E81" t="s">
         <v>17</v>
       </c>
       <c r="F81" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G81" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3187,45 +3361,45 @@
         <v>26</v>
       </c>
       <c r="B82" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C82">
         <v>56</v>
       </c>
       <c r="D82" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E82" t="s">
         <v>17</v>
       </c>
       <c r="F82" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G82" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B83" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C83" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D83" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E83" t="s">
         <v>17</v>
       </c>
       <c r="F83" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G83" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3233,22 +3407,22 @@
         <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C84">
         <v>56</v>
       </c>
       <c r="D84" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E84" t="s">
         <v>17</v>
       </c>
       <c r="F84" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G84" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3256,22 +3430,22 @@
         <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C85">
         <v>56</v>
       </c>
       <c r="D85" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E85" t="s">
         <v>17</v>
       </c>
       <c r="F85" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G85" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -3279,22 +3453,22 @@
         <v>7</v>
       </c>
       <c r="B86" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C86">
         <v>68</v>
       </c>
       <c r="D86" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E86" t="s">
         <v>17</v>
       </c>
       <c r="F86" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G86" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -3302,114 +3476,114 @@
         <v>7</v>
       </c>
       <c r="B87" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C87">
         <v>68</v>
       </c>
       <c r="D87" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E87" t="s">
         <v>17</v>
       </c>
       <c r="F87" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G87" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B88" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C88">
         <v>56</v>
       </c>
       <c r="D88" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E88" t="s">
         <v>17</v>
       </c>
       <c r="F88" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G88" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C89">
         <v>56</v>
       </c>
       <c r="D89" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E89" t="s">
         <v>17</v>
       </c>
       <c r="F89" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G89" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B90" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C90">
         <v>62</v>
       </c>
       <c r="D90" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E90" t="s">
         <v>17</v>
       </c>
       <c r="F90" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G90" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C91" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D91" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E91" t="s">
         <v>17</v>
       </c>
       <c r="F91" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G91" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -3417,22 +3591,22 @@
         <v>30</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C92">
         <v>62</v>
       </c>
       <c r="D92" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E92" t="s">
         <v>17</v>
       </c>
       <c r="F92" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G92" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -3440,22 +3614,22 @@
         <v>30</v>
       </c>
       <c r="B93" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C93">
         <v>74</v>
       </c>
       <c r="D93" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E93" t="s">
         <v>17</v>
       </c>
       <c r="F93" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G93" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3463,22 +3637,22 @@
         <v>30</v>
       </c>
       <c r="B94" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C94">
         <v>86</v>
       </c>
       <c r="D94" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E94" t="s">
         <v>17</v>
       </c>
       <c r="F94" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G94" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -3486,22 +3660,22 @@
         <v>30</v>
       </c>
       <c r="B95" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C95" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D95" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E95" t="s">
         <v>17</v>
       </c>
       <c r="F95" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G95" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -3509,22 +3683,22 @@
         <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C96">
         <v>56</v>
       </c>
       <c r="D96" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E96" t="s">
         <v>17</v>
       </c>
       <c r="F96" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G96" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -3532,82 +3706,82 @@
         <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C97">
         <v>62</v>
       </c>
       <c r="D97" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E97" t="s">
         <v>17</v>
       </c>
       <c r="F97" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B98" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C98">
         <v>50</v>
       </c>
       <c r="D98" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E98" t="s">
         <v>17</v>
       </c>
       <c r="F98" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G98" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B99" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C99">
         <v>56</v>
       </c>
       <c r="D99" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E99" t="s">
         <v>17</v>
       </c>
       <c r="F99" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G99" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B100" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C100">
         <v>56</v>
       </c>
       <c r="D100" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E100" t="s">
         <v>17</v>
@@ -3616,7 +3790,7 @@
         <v>18</v>
       </c>
       <c r="G100" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3624,13 +3798,13 @@
         <v>7</v>
       </c>
       <c r="B101" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C101" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D101" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E101" t="s">
         <v>17</v>
@@ -3639,7 +3813,7 @@
         <v>18</v>
       </c>
       <c r="G101" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3647,13 +3821,13 @@
         <v>7</v>
       </c>
       <c r="B102" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C102">
         <v>50</v>
       </c>
       <c r="D102" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E102" t="s">
         <v>17</v>
@@ -3662,21 +3836,21 @@
         <v>18</v>
       </c>
       <c r="G102" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B103" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C103">
         <v>56</v>
       </c>
       <c r="D103" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E103" t="s">
         <v>17</v>
@@ -3685,21 +3859,21 @@
         <v>18</v>
       </c>
       <c r="G103" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B104" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C104" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E104" t="s">
         <v>17</v>
@@ -3708,21 +3882,21 @@
         <v>18</v>
       </c>
       <c r="G104" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B105" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C105">
         <v>56</v>
       </c>
       <c r="D105" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E105" t="s">
         <v>17</v>
@@ -3731,21 +3905,21 @@
         <v>18</v>
       </c>
       <c r="G105" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B106" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C106">
         <v>56</v>
       </c>
       <c r="D106" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E106" t="s">
         <v>17</v>
@@ -3754,21 +3928,21 @@
         <v>18</v>
       </c>
       <c r="G106" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B107" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C107">
         <v>50</v>
       </c>
       <c r="D107" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E107" t="s">
         <v>17</v>
@@ -3777,21 +3951,21 @@
         <v>18</v>
       </c>
       <c r="G107" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B108" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C108">
         <v>56</v>
       </c>
       <c r="D108" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E108" t="s">
         <v>17</v>
@@ -3800,7 +3974,7 @@
         <v>18</v>
       </c>
       <c r="G108" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3808,13 +3982,13 @@
         <v>7</v>
       </c>
       <c r="B109" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C109">
         <v>50</v>
       </c>
       <c r="D109" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E109" t="s">
         <v>17</v>
@@ -3823,7 +3997,7 @@
         <v>18</v>
       </c>
       <c r="G109" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3831,13 +4005,13 @@
         <v>7</v>
       </c>
       <c r="B110" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C110" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E110" t="s">
         <v>17</v>
@@ -3846,7 +4020,7 @@
         <v>18</v>
       </c>
       <c r="G110" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3854,13 +4028,13 @@
         <v>7</v>
       </c>
       <c r="B111" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C111" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D111" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E111" t="s">
         <v>17</v>
@@ -3869,7 +4043,7 @@
         <v>18</v>
       </c>
       <c r="G111" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3877,13 +4051,13 @@
         <v>7</v>
       </c>
       <c r="B112" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C112" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D112" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E112" t="s">
         <v>17</v>
@@ -3892,21 +4066,21 @@
         <v>18</v>
       </c>
       <c r="G112" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B113" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C113">
         <v>56</v>
       </c>
       <c r="D113" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E113" t="s">
         <v>17</v>
@@ -3915,7 +4089,7 @@
         <v>18</v>
       </c>
       <c r="G113" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3923,13 +4097,13 @@
         <v>7</v>
       </c>
       <c r="B114" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C114">
         <v>62</v>
       </c>
       <c r="D114" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E114" t="s">
         <v>17</v>
@@ -3938,7 +4112,7 @@
         <v>18</v>
       </c>
       <c r="G114" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3946,13 +4120,13 @@
         <v>7</v>
       </c>
       <c r="B115" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C115" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D115" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E115" t="s">
         <v>17</v>
@@ -3961,7 +4135,7 @@
         <v>18</v>
       </c>
       <c r="G115" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3969,13 +4143,13 @@
         <v>7</v>
       </c>
       <c r="B116" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C116" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D116" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E116" t="s">
         <v>17</v>
@@ -3984,7 +4158,7 @@
         <v>18</v>
       </c>
       <c r="G116" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3992,13 +4166,13 @@
         <v>7</v>
       </c>
       <c r="B117" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C117" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D117" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E117" t="s">
         <v>17</v>
@@ -4007,21 +4181,21 @@
         <v>18</v>
       </c>
       <c r="G117" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B118" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C118">
         <v>62</v>
       </c>
       <c r="D118" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E118" t="s">
         <v>17</v>
@@ -4030,21 +4204,21 @@
         <v>18</v>
       </c>
       <c r="G118" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B119" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C119">
         <v>62</v>
       </c>
       <c r="D119" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E119" t="s">
         <v>17</v>
@@ -4053,21 +4227,21 @@
         <v>18</v>
       </c>
       <c r="G119" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B120" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C120">
         <v>62</v>
       </c>
       <c r="D120" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E120" t="s">
         <v>17</v>
@@ -4076,21 +4250,21 @@
         <v>18</v>
       </c>
       <c r="G120" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B121" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C121">
         <v>68</v>
       </c>
       <c r="D121" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E121" t="s">
         <v>17</v>
@@ -4099,21 +4273,21 @@
         <v>18</v>
       </c>
       <c r="G121" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B122" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C122">
         <v>62</v>
       </c>
       <c r="D122" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E122" t="s">
         <v>17</v>
@@ -4122,7 +4296,7 @@
         <v>18</v>
       </c>
       <c r="G122" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4130,91 +4304,91 @@
         <v>7</v>
       </c>
       <c r="B123" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C123">
         <v>68</v>
       </c>
       <c r="D123" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E123" t="s">
         <v>17</v>
       </c>
       <c r="F123" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G123" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B124" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C124">
         <v>68</v>
       </c>
       <c r="D124" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E124" t="s">
         <v>17</v>
       </c>
       <c r="F124" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G124" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B125" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C125">
         <v>68</v>
       </c>
       <c r="D125" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E125" t="s">
         <v>17</v>
       </c>
       <c r="F125" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G125" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B126" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C126">
         <v>68</v>
       </c>
       <c r="D126" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E126" t="s">
         <v>17</v>
       </c>
       <c r="F126" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G126" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -4222,45 +4396,45 @@
         <v>7</v>
       </c>
       <c r="B127" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C127">
         <v>68</v>
       </c>
       <c r="D127" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E127" t="s">
         <v>17</v>
       </c>
       <c r="F127" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G127" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B128" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C128">
         <v>74</v>
       </c>
       <c r="D128" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E128" t="s">
         <v>17</v>
       </c>
       <c r="F128" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G128" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -4268,22 +4442,22 @@
         <v>7</v>
       </c>
       <c r="B129" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C129">
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E129" t="s">
         <v>17</v>
       </c>
       <c r="F129" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G129" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4291,206 +4465,873 @@
         <v>7</v>
       </c>
       <c r="B130" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C130">
         <v>68</v>
       </c>
       <c r="D130" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E130" t="s">
         <v>17</v>
       </c>
       <c r="F130" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G130" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B131" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C131">
         <v>56</v>
       </c>
       <c r="D131" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E131" t="s">
         <v>17</v>
       </c>
       <c r="F131" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G131" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B132" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C132">
         <v>50</v>
       </c>
       <c r="D132" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E132" t="s">
         <v>17</v>
       </c>
       <c r="F132" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G132" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B133" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C133">
         <v>80</v>
       </c>
       <c r="D133" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E133" t="s">
         <v>17</v>
       </c>
       <c r="F133" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G133" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B134" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C134" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D134" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E134" t="s">
         <v>17</v>
       </c>
       <c r="F134" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G134" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B135" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C135">
         <v>74</v>
       </c>
       <c r="D135" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E135" t="s">
         <v>17</v>
       </c>
       <c r="F135" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G135" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B136" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C136">
         <v>80</v>
       </c>
       <c r="D136" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E136" t="s">
         <v>17</v>
       </c>
       <c r="F136" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G136" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B137" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C137">
         <v>86</v>
       </c>
       <c r="D137" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E137" t="s">
         <v>17</v>
       </c>
       <c r="F137" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G137" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B138" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C138" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D138" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E138" t="s">
         <v>17</v>
       </c>
       <c r="F138" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G138" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>160</v>
+      </c>
+      <c r="B139" t="s">
+        <v>66</v>
+      </c>
+      <c r="C139">
+        <v>22</v>
+      </c>
+      <c r="D139" t="s">
+        <v>317</v>
+      </c>
+      <c r="E139" t="s">
+        <v>17</v>
+      </c>
+      <c r="F139" t="s">
+        <v>318</v>
+      </c>
+      <c r="G139" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
+        <v>160</v>
+      </c>
+      <c r="B140" t="s">
+        <v>320</v>
+      </c>
+      <c r="C140">
+        <v>23</v>
+      </c>
+      <c r="D140" t="s">
+        <v>321</v>
+      </c>
+      <c r="E140" t="s">
+        <v>17</v>
+      </c>
+      <c r="F140" t="s">
+        <v>318</v>
+      </c>
+      <c r="G140" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
+        <v>33</v>
+      </c>
+      <c r="B141" t="s">
+        <v>322</v>
+      </c>
+      <c r="C141">
+        <v>92</v>
+      </c>
+      <c r="D141" t="s">
+        <v>323</v>
+      </c>
+      <c r="E141" t="s">
+        <v>17</v>
+      </c>
+      <c r="F141" t="s">
+        <v>318</v>
+      </c>
+      <c r="G141" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
+        <v>33</v>
+      </c>
+      <c r="B142" t="s">
+        <v>324</v>
+      </c>
+      <c r="C142">
+        <v>92</v>
+      </c>
+      <c r="D142" t="s">
+        <v>325</v>
+      </c>
+      <c r="E142" t="s">
+        <v>17</v>
+      </c>
+      <c r="F142" t="s">
+        <v>318</v>
+      </c>
+      <c r="G142" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
+        <v>33</v>
+      </c>
+      <c r="B143" t="s">
+        <v>326</v>
+      </c>
+      <c r="C143">
+        <v>92</v>
+      </c>
+      <c r="D143" t="s">
+        <v>327</v>
+      </c>
+      <c r="E143" t="s">
+        <v>17</v>
+      </c>
+      <c r="F143" t="s">
+        <v>318</v>
+      </c>
+      <c r="G143" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" t="s">
+        <v>33</v>
+      </c>
+      <c r="B144" t="s">
+        <v>328</v>
+      </c>
+      <c r="C144" t="s">
+        <v>329</v>
+      </c>
+      <c r="D144" t="s">
+        <v>330</v>
+      </c>
+      <c r="E144" t="s">
+        <v>17</v>
+      </c>
+      <c r="F144" t="s">
+        <v>318</v>
+      </c>
+      <c r="G144" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>33</v>
+      </c>
+      <c r="B145" t="s">
+        <v>331</v>
+      </c>
+      <c r="C145">
+        <v>86</v>
+      </c>
+      <c r="D145" t="s">
+        <v>332</v>
+      </c>
+      <c r="E145" t="s">
+        <v>17</v>
+      </c>
+      <c r="F145" t="s">
+        <v>318</v>
+      </c>
+      <c r="G145" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>26</v>
+      </c>
+      <c r="B146" t="s">
+        <v>326</v>
+      </c>
+      <c r="C146">
+        <v>80</v>
+      </c>
+      <c r="D146" t="s">
+        <v>333</v>
+      </c>
+      <c r="E146" t="s">
+        <v>17</v>
+      </c>
+      <c r="F146" t="s">
+        <v>318</v>
+      </c>
+      <c r="G146" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>26</v>
+      </c>
+      <c r="B147" t="s">
+        <v>334</v>
+      </c>
+      <c r="C147" t="s">
+        <v>230</v>
+      </c>
+      <c r="D147" t="s">
+        <v>335</v>
+      </c>
+      <c r="E147" t="s">
+        <v>17</v>
+      </c>
+      <c r="F147" t="s">
+        <v>318</v>
+      </c>
+      <c r="G147" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>65</v>
+      </c>
+      <c r="B148" t="s">
+        <v>336</v>
+      </c>
+      <c r="C148">
+        <v>68</v>
+      </c>
+      <c r="D148" t="s">
+        <v>337</v>
+      </c>
+      <c r="E148" t="s">
+        <v>17</v>
+      </c>
+      <c r="F148" t="s">
+        <v>121</v>
+      </c>
+      <c r="G148" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>164</v>
+      </c>
+      <c r="B149" t="s">
+        <v>338</v>
+      </c>
+      <c r="C149">
+        <v>74</v>
+      </c>
+      <c r="D149" t="s">
+        <v>339</v>
+      </c>
+      <c r="E149" t="s">
+        <v>17</v>
+      </c>
+      <c r="F149" t="s">
+        <v>121</v>
+      </c>
+      <c r="G149" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>164</v>
+      </c>
+      <c r="B150" t="s">
+        <v>340</v>
+      </c>
+      <c r="C150">
+        <v>62</v>
+      </c>
+      <c r="D150" t="s">
+        <v>341</v>
+      </c>
+      <c r="E150" t="s">
+        <v>10</v>
+      </c>
+      <c r="F150" t="s">
+        <v>11</v>
+      </c>
+      <c r="G150" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>40</v>
+      </c>
+      <c r="B151" t="s">
+        <v>342</v>
+      </c>
+      <c r="C151">
+        <v>68</v>
+      </c>
+      <c r="D151" t="s">
+        <v>343</v>
+      </c>
+      <c r="E151" t="s">
+        <v>17</v>
+      </c>
+      <c r="F151" t="s">
+        <v>18</v>
+      </c>
+      <c r="G151" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>7</v>
+      </c>
+      <c r="B152" t="s">
+        <v>344</v>
+      </c>
+      <c r="C152">
+        <v>68</v>
+      </c>
+      <c r="D152" t="s">
+        <v>345</v>
+      </c>
+      <c r="E152" t="s">
+        <v>17</v>
+      </c>
+      <c r="F152" t="s">
+        <v>18</v>
+      </c>
+      <c r="G152" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>7</v>
+      </c>
+      <c r="B153" t="s">
+        <v>346</v>
+      </c>
+      <c r="C153">
+        <v>62</v>
+      </c>
+      <c r="D153" t="s">
+        <v>347</v>
+      </c>
+      <c r="E153" t="s">
+        <v>10</v>
+      </c>
+      <c r="F153" t="s">
+        <v>11</v>
+      </c>
+      <c r="G153" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>169</v>
+      </c>
+      <c r="B154" t="s">
+        <v>348</v>
+      </c>
+      <c r="C154">
+        <v>68</v>
+      </c>
+      <c r="D154" t="s">
+        <v>349</v>
+      </c>
+      <c r="E154" t="s">
+        <v>17</v>
+      </c>
+      <c r="F154" t="s">
+        <v>18</v>
+      </c>
+      <c r="G154" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>164</v>
+      </c>
+      <c r="B155" t="s">
+        <v>350</v>
+      </c>
+      <c r="C155">
+        <v>68</v>
+      </c>
+      <c r="D155" t="s">
+        <v>351</v>
+      </c>
+      <c r="E155" t="s">
+        <v>17</v>
+      </c>
+      <c r="F155" t="s">
+        <v>18</v>
+      </c>
+      <c r="G155" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" t="s">
+        <v>164</v>
+      </c>
+      <c r="B156" t="s">
+        <v>186</v>
+      </c>
+      <c r="C156">
+        <v>56</v>
+      </c>
+      <c r="D156" t="s">
+        <v>352</v>
+      </c>
+      <c r="E156" t="s">
+        <v>17</v>
+      </c>
+      <c r="F156" t="s">
+        <v>18</v>
+      </c>
+      <c r="G156" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" t="s">
+        <v>40</v>
+      </c>
+      <c r="B157" t="s">
+        <v>353</v>
+      </c>
+      <c r="C157">
+        <v>68</v>
+      </c>
+      <c r="D157" t="s">
+        <v>354</v>
+      </c>
+      <c r="E157" t="s">
+        <v>17</v>
+      </c>
+      <c r="F157" t="s">
+        <v>18</v>
+      </c>
+      <c r="G157" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" t="s">
+        <v>169</v>
+      </c>
+      <c r="B158" t="s">
+        <v>355</v>
+      </c>
+      <c r="C158">
+        <v>62</v>
+      </c>
+      <c r="D158" t="s">
+        <v>356</v>
+      </c>
+      <c r="E158" t="s">
+        <v>10</v>
+      </c>
+      <c r="F158" t="s">
+        <v>11</v>
+      </c>
+      <c r="G158" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>40</v>
+      </c>
+      <c r="B159" t="s">
+        <v>357</v>
+      </c>
+      <c r="C159">
+        <v>74</v>
+      </c>
+      <c r="D159" t="s">
+        <v>358</v>
+      </c>
+      <c r="E159" t="s">
+        <v>17</v>
+      </c>
+      <c r="F159" t="s">
+        <v>18</v>
+      </c>
+      <c r="G159" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>40</v>
+      </c>
+      <c r="B160" t="s">
+        <v>359</v>
+      </c>
+      <c r="C160">
+        <v>68</v>
+      </c>
+      <c r="D160" t="s">
+        <v>360</v>
+      </c>
+      <c r="E160" t="s">
+        <v>17</v>
+      </c>
+      <c r="F160" t="s">
+        <v>18</v>
+      </c>
+      <c r="G160" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>164</v>
+      </c>
+      <c r="B161" t="s">
+        <v>361</v>
+      </c>
+      <c r="C161">
+        <v>68</v>
+      </c>
+      <c r="D161" t="s">
+        <v>362</v>
+      </c>
+      <c r="E161" t="s">
+        <v>17</v>
+      </c>
+      <c r="F161" t="s">
+        <v>18</v>
+      </c>
+      <c r="G161" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>7</v>
+      </c>
+      <c r="B162" t="s">
+        <v>363</v>
+      </c>
+      <c r="C162">
+        <v>86</v>
+      </c>
+      <c r="D162" t="s">
+        <v>364</v>
+      </c>
+      <c r="E162" t="s">
+        <v>17</v>
+      </c>
+      <c r="F162" t="s">
+        <v>18</v>
+      </c>
+      <c r="G162" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163" t="s">
+        <v>365</v>
+      </c>
+      <c r="C163">
+        <v>56</v>
+      </c>
+      <c r="D163" t="s">
+        <v>366</v>
+      </c>
+      <c r="E163" t="s">
+        <v>17</v>
+      </c>
+      <c r="F163" t="s">
+        <v>18</v>
+      </c>
+      <c r="G163" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" t="s">
+        <v>40</v>
+      </c>
+      <c r="B164" t="s">
+        <v>89</v>
+      </c>
+      <c r="C164">
+        <v>74</v>
+      </c>
+      <c r="D164" t="s">
+        <v>367</v>
+      </c>
+      <c r="E164" t="s">
+        <v>17</v>
+      </c>
+      <c r="F164" t="s">
+        <v>18</v>
+      </c>
+      <c r="G164" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" t="s">
+        <v>40</v>
+      </c>
+      <c r="B165" t="s">
+        <v>368</v>
+      </c>
+      <c r="C165">
+        <v>68</v>
+      </c>
+      <c r="D165" t="s">
+        <v>369</v>
+      </c>
+      <c r="E165" t="s">
+        <v>17</v>
+      </c>
+      <c r="F165" t="s">
+        <v>18</v>
+      </c>
+      <c r="G165" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" t="s">
+        <v>40</v>
+      </c>
+      <c r="B166" t="s">
+        <v>370</v>
+      </c>
+      <c r="C166" t="s">
+        <v>189</v>
+      </c>
+      <c r="D166" t="s">
+        <v>371</v>
+      </c>
+      <c r="E166" t="s">
+        <v>17</v>
+      </c>
+      <c r="F166" t="s">
+        <v>18</v>
+      </c>
+      <c r="G166" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167" t="s">
+        <v>258</v>
+      </c>
+      <c r="C167" t="s">
+        <v>372</v>
+      </c>
+      <c r="D167" t="s">
+        <v>373</v>
+      </c>
+      <c r="E167" t="s">
+        <v>17</v>
+      </c>
+      <c r="F167" t="s">
+        <v>18</v>
+      </c>
+      <c r="G167" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>